<commit_message>
Exportación de excel semicompleta
</commit_message>
<xml_diff>
--- a/view/Asistencias/Contreras Oscar.xlsx
+++ b/view/Asistencias/Contreras Oscar.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>Contreras Oscar</t>
   </si>
@@ -26,25 +26,178 @@
     <t>Reporte de Asistencias IN Consulting</t>
   </si>
   <si>
-    <t>16-Jun-2023</t>
+    <t>17/Jun/2023</t>
+  </si>
+  <si>
+    <t>NSS: 654321965432</t>
+  </si>
+  <si>
+    <t>Departamento: JEFE DE COCINA</t>
+  </si>
+  <si>
+    <t>Horas esperadas</t>
+  </si>
+  <si>
+    <t>Horas registradas</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
+  </si>
+  <si>
+    <t>48h 0min</t>
+  </si>
+  <si>
+    <t>71h 46min</t>
+  </si>
+  <si>
+    <t>23h 46min</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Esperado</t>
+  </si>
+  <si>
+    <t>Inicio - Fin</t>
+  </si>
+  <si>
+    <t>Pausa</t>
+  </si>
+  <si>
+    <t>Registrado</t>
+  </si>
+  <si>
+    <t>Comentario</t>
+  </si>
+  <si>
+    <t>RFC: COFO911219925</t>
   </si>
   <si>
     <t>CURP: COFO911219HMNNLS06</t>
   </si>
   <si>
-    <t>Departamento: JEFE DE COCINA</t>
-  </si>
-  <si>
-    <t>Nombre: Contreras Oscar</t>
-  </si>
-  <si>
-    <t>RFC: COFO911219925</t>
-  </si>
-  <si>
     <t>Empresa: AVOCADOS PHAWA</t>
   </si>
   <si>
     <t>Puesto: Auxiliar de Almacen de Caja de Campo</t>
+  </si>
+  <si>
+    <t>* Ausencias y festivos</t>
+  </si>
+  <si>
+    <t>07:33:00 - 16:37:00</t>
+  </si>
+  <si>
+    <t>Lu</t>
+  </si>
+  <si>
+    <t>05/Jun/2023</t>
+  </si>
+  <si>
+    <t>0h 48min</t>
+  </si>
+  <si>
+    <t>8h 16min</t>
+  </si>
+  <si>
+    <t>08:25:00 - 16:37:00</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>06/Jun/2023</t>
+  </si>
+  <si>
+    <t>0h 58min</t>
+  </si>
+  <si>
+    <t>7h 14min</t>
+  </si>
+  <si>
+    <t>07:37:00 - 16:37:00</t>
+  </si>
+  <si>
+    <t>no alcance a llegar</t>
+  </si>
+  <si>
+    <t>Mi</t>
+  </si>
+  <si>
+    <t>07/Jun/2023</t>
+  </si>
+  <si>
+    <t>1h 8min</t>
+  </si>
+  <si>
+    <t>7h 52min</t>
+  </si>
+  <si>
+    <t>08:00:00 - 17:11:00</t>
+  </si>
+  <si>
+    <t>Ju</t>
+  </si>
+  <si>
+    <t>08/Jun/2023</t>
+  </si>
+  <si>
+    <t>1h 18min</t>
+  </si>
+  <si>
+    <t>7h 53min</t>
+  </si>
+  <si>
+    <t>07:55:00 - 17:58:00</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>Vi</t>
+  </si>
+  <si>
+    <t>09/Jun/2023</t>
+  </si>
+  <si>
+    <t>0h 40min</t>
+  </si>
+  <si>
+    <t>9h 23min</t>
+  </si>
+  <si>
+    <t>12/Jun/2023</t>
+  </si>
+  <si>
+    <t>7h 32min</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>13/Jun/2023</t>
+  </si>
+  <si>
+    <t>07:47:00 - 17:37:00</t>
+  </si>
+  <si>
+    <t>14/Jun/2023</t>
+  </si>
+  <si>
+    <t>9h 10min</t>
+  </si>
+  <si>
+    <t>estaba tomado el centro</t>
+  </si>
+  <si>
+    <t>15/Jun/2023</t>
+  </si>
+  <si>
+    <t>6h 54min</t>
   </si>
 </sst>
 </file>
@@ -81,7 +234,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,8 +247,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ff52dc96"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ffeeab59"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -147,6 +312,21 @@
       <left style="thin">
         <color rgb="ff949494"/>
       </left>
+      <right style="thin">
+        <color rgb="ff949494"/>
+      </right>
+      <top style="thin">
+        <color rgb="ff949494"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="ff949494"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="ff949494"/>
+      </left>
       <right/>
       <top style="thin">
         <color rgb="ff949494"/>
@@ -169,15 +349,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -185,12 +367,14 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,21 +674,21 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I20" sqref="I20:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -519,24 +703,24 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -557,52 +741,342 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="10">
+      <c r="B9" s="12">
         <v>2023</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I20:L20"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
+    <oddHeader>&amp;L&amp;G</oddHeader>
     <oddFooter/>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <legacyDrawingHF r:id="rId_headerfooter_vml1"/>
   <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exportación de datos excel
</commit_message>
<xml_diff>
--- a/view/Asistencias/Contreras Oscar.xlsx
+++ b/view/Asistencias/Contreras Oscar.xlsx
@@ -15,42 +15,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
   <si>
     <t>Contreras Oscar</t>
   </si>
   <si>
+    <t>RFC: COFO911219925</t>
+  </si>
+  <si>
+    <t>CURP: COFO911219HMNNLS06</t>
+  </si>
+  <si>
+    <t>NSS: 654321965432</t>
+  </si>
+  <si>
+    <t>Empresa: AVOCADOS PHAWA</t>
+  </si>
+  <si>
+    <t>Puesto: Auxiliar de Almacen de Caja de Campo</t>
+  </si>
+  <si>
+    <t>Departamento: JEFE DE COCINA</t>
+  </si>
+  <si>
     <t>Junio</t>
   </si>
   <si>
+    <t>Horas esperadas (2da quincena)</t>
+  </si>
+  <si>
+    <t>117h 0min</t>
+  </si>
+  <si>
+    <t>Horas esperadas (1er quincena)</t>
+  </si>
+  <si>
+    <t>Horas registradas</t>
+  </si>
+  <si>
+    <t>7h 32min</t>
+  </si>
+  <si>
     <t>Reporte de Asistencias IN Consulting</t>
   </si>
   <si>
-    <t>17/Jun/2023</t>
-  </si>
-  <si>
-    <t>NSS: 654321965432</t>
-  </si>
-  <si>
-    <t>Departamento: JEFE DE COCINA</t>
-  </si>
-  <si>
-    <t>Horas esperadas</t>
-  </si>
-  <si>
-    <t>Horas registradas</t>
+    <t>20/Jun/2023</t>
   </si>
   <si>
     <t>Diferencia</t>
   </si>
   <si>
-    <t>48h 0min</t>
-  </si>
-  <si>
-    <t>71h 46min</t>
-  </si>
-  <si>
-    <t>23h 46min</t>
+    <t>109h 28min</t>
   </si>
   <si>
     <t>Fecha</t>
@@ -62,7 +77,7 @@
     <t>Inicio - Fin</t>
   </si>
   <si>
-    <t>Pausa</t>
+    <t>Descanso: Inicio - Fin</t>
   </si>
   <si>
     <t>Registrado</t>
@@ -71,133 +86,193 @@
     <t>Comentario</t>
   </si>
   <si>
-    <t>RFC: COFO911219925</t>
-  </si>
-  <si>
-    <t>CURP: COFO911219HMNNLS06</t>
-  </si>
-  <si>
-    <t>Empresa: AVOCADOS PHAWA</t>
-  </si>
-  <si>
-    <t>Puesto: Auxiliar de Almacen de Caja de Campo</t>
-  </si>
-  <si>
     <t>* Ausencias y festivos</t>
   </si>
   <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>9h 0min</t>
+  </si>
+  <si>
+    <t>Ju</t>
+  </si>
+  <si>
+    <t>01/06/2023</t>
+  </si>
+  <si>
+    <t>Vi</t>
+  </si>
+  <si>
+    <t>02/06/2023</t>
+  </si>
+  <si>
+    <t>Sá</t>
+  </si>
+  <si>
+    <t>03/06/2023</t>
+  </si>
+  <si>
+    <t>Do</t>
+  </si>
+  <si>
+    <t>04/06/2023</t>
+  </si>
+  <si>
     <t>07:33:00 - 16:37:00</t>
   </si>
   <si>
+    <t>14:32:00 - 15:20:00</t>
+  </si>
+  <si>
+    <t>8h 16min</t>
+  </si>
+  <si>
     <t>Lu</t>
   </si>
   <si>
-    <t>05/Jun/2023</t>
-  </si>
-  <si>
-    <t>0h 48min</t>
-  </si>
-  <si>
-    <t>8h 16min</t>
+    <t>05/06/2023</t>
   </si>
   <si>
     <t>08:25:00 - 16:37:00</t>
   </si>
   <si>
-    <t>check</t>
+    <t>14:32:00 - 15:30:00</t>
+  </si>
+  <si>
+    <t>7h 14min</t>
   </si>
   <si>
     <t>Ma</t>
   </si>
   <si>
-    <t>06/Jun/2023</t>
-  </si>
-  <si>
-    <t>0h 58min</t>
-  </si>
-  <si>
-    <t>7h 14min</t>
+    <t>06/06/2023</t>
   </si>
   <si>
     <t>07:37:00 - 16:37:00</t>
   </si>
   <si>
-    <t>no alcance a llegar</t>
+    <t>14:32:00 - 15:40:00</t>
+  </si>
+  <si>
+    <t>7h 52min</t>
   </si>
   <si>
     <t>Mi</t>
   </si>
   <si>
-    <t>07/Jun/2023</t>
-  </si>
-  <si>
-    <t>1h 8min</t>
-  </si>
-  <si>
-    <t>7h 52min</t>
+    <t>07/06/2023</t>
   </si>
   <si>
     <t>08:00:00 - 17:11:00</t>
   </si>
   <si>
-    <t>Ju</t>
-  </si>
-  <si>
-    <t>08/Jun/2023</t>
-  </si>
-  <si>
-    <t>1h 18min</t>
+    <t>14:32:00 - 15:50:00</t>
   </si>
   <si>
     <t>7h 53min</t>
   </si>
   <si>
+    <t>08/06/2023</t>
+  </si>
+  <si>
     <t>07:55:00 - 17:58:00</t>
   </si>
   <si>
+    <t>14:32:00 - 15:12:00</t>
+  </si>
+  <si>
+    <t>9h 23min</t>
+  </si>
+  <si>
     <t>Prueba</t>
   </si>
   <si>
-    <t>Vi</t>
-  </si>
-  <si>
-    <t>09/Jun/2023</t>
-  </si>
-  <si>
-    <t>0h 40min</t>
-  </si>
-  <si>
-    <t>9h 23min</t>
-  </si>
-  <si>
-    <t>12/Jun/2023</t>
-  </si>
-  <si>
-    <t>7h 32min</t>
+    <t>09/06/2023</t>
+  </si>
+  <si>
+    <t>00:00:00 - 00:00:00</t>
+  </si>
+  <si>
+    <t>0h 0min</t>
+  </si>
+  <si>
+    <t>10/06/2023</t>
+  </si>
+  <si>
+    <t>11/06/2023</t>
+  </si>
+  <si>
+    <t>12/06/2023</t>
+  </si>
+  <si>
+    <t>13/06/2023</t>
+  </si>
+  <si>
+    <t>07:47:00 - 17:37:00</t>
+  </si>
+  <si>
+    <t>9h 10min</t>
+  </si>
+  <si>
+    <t>14/06/2023</t>
+  </si>
+  <si>
+    <t>6h 54min</t>
+  </si>
+  <si>
+    <t>estaba tomado el centro</t>
+  </si>
+  <si>
+    <t>15/06/2023</t>
   </si>
   <si>
     <t>prueba</t>
   </si>
   <si>
-    <t>13/Jun/2023</t>
-  </si>
-  <si>
-    <t>07:47:00 - 17:37:00</t>
-  </si>
-  <si>
-    <t>14/Jun/2023</t>
-  </si>
-  <si>
-    <t>9h 10min</t>
-  </si>
-  <si>
-    <t>estaba tomado el centro</t>
-  </si>
-  <si>
-    <t>15/Jun/2023</t>
-  </si>
-  <si>
-    <t>6h 54min</t>
+    <t>16/06/2023</t>
+  </si>
+  <si>
+    <t>17/06/2023</t>
+  </si>
+  <si>
+    <t>18/06/2023</t>
+  </si>
+  <si>
+    <t>19/06/2023</t>
+  </si>
+  <si>
+    <t>20/06/2023</t>
+  </si>
+  <si>
+    <t>21/06/2023</t>
+  </si>
+  <si>
+    <t>22/06/2023</t>
+  </si>
+  <si>
+    <t>23/06/2023</t>
+  </si>
+  <si>
+    <t>24/06/2023</t>
+  </si>
+  <si>
+    <t>25/06/2023</t>
+  </si>
+  <si>
+    <t>26/06/2023</t>
+  </si>
+  <si>
+    <t>27/06/2023</t>
+  </si>
+  <si>
+    <t>28/06/2023</t>
+  </si>
+  <si>
+    <t>29/06/2023</t>
+  </si>
+  <si>
+    <t>30/06/2023</t>
   </si>
 </sst>
 </file>
@@ -249,7 +324,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="ff52dc96"/>
+        <fgColor rgb="ffbababa"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -260,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -345,11 +420,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
@@ -375,6 +459,8 @@
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,13 +760,21 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I20" sqref="I20:L20"/>
+      <selection activeCell="B36" sqref="B36:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="2" max="2" width="3" customWidth="true" style="0"/>
+    <col min="3" max="3" width="11" customWidth="true" style="0"/>
+    <col min="4" max="4" width="10" customWidth="true" style="0"/>
+    <col min="8" max="8" width="10" customWidth="true" style="0"/>
+    <col min="9" max="9" width="10" customWidth="true" style="0"/>
+    <col min="12" max="12" width="20" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:12">
       <c r="B2" s="8" t="s">
@@ -689,7 +783,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="L3" s="9" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -704,35 +798,35 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="10" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -742,24 +836,26 @@
     </row>
     <row r="8" spans="1:12">
       <c r="B8" s="11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4" t="s">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K8" s="4"/>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" s="12">
@@ -770,169 +866,145 @@
         <v>9</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="K9" s="5"/>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="J12"/>
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+        <v>24</v>
+      </c>
+      <c r="J13"/>
     </row>
     <row r="14" spans="1:12">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+        <v>24</v>
+      </c>
+      <c r="J14"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="B15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:12">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -940,130 +1012,621 @@
     </row>
     <row r="17" spans="1:12">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
+        <v>45</v>
+      </c>
+      <c r="I18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12">
       <c r="B19" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
+        <v>51</v>
+      </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12">
       <c r="B20" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="B22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="B26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="G20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="B29" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="B36" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38" t="s">
+        <v>24</v>
+      </c>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:E3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="G7:L7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="J11:L11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="J12:L12"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:L13"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:L16"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J17:L17"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="J18:L18"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J19:L19"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="J41:L41"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>